<commit_message>
Update old information architecture
</commit_message>
<xml_diff>
--- a/_docs_readme/information-architecture_original.xlsx
+++ b/_docs_readme/information-architecture_original.xlsx
@@ -8,8 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FilipaGomes/Filipa_Ensino/PG_DXD/Projecto DXD/redesign_fbaul/06_prototipo-github/_docs_readme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{14381865-FDF0-B040-A075-7716B32C9247}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Dw0VL6sl/J7Plr/X8PoB27DIrfLkOvEFTtC7YcCPLRNvkMliT+AkXjM05v3nVmjMbeGCMC28LhydIgcqsSRtAQ==" workbookSaltValue="qfsXx3Bv5WBuS8fYzLjGYw==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{18F169EF-034F-F045-97CA-AF4AA91C0A1F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="7mmU6vbSTN5HNPRZJykSDZzCyFT/fj5QWVDukKr+OBTMdbyWOPn+g4ZWyZNV8FzmydhsKKrAJJjlUz3ELZULLA==" workbookSaltValue="TcpsNes1jcX/gvj6MMcCVw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="500" windowWidth="28640" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>